<commit_message>
added metadata file from Tomo
</commit_message>
<xml_diff>
--- a/metadata/batch_info_ALCL.xlsx
+++ b/metadata/batch_info_ALCL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\davidson\ALCL\single_cell\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/putriramadani/Documents/GitHub/scRNAseq_ALCL_Thymus_RLN/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A2010B-577A-4D7E-9CAD-A6F9145A47F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2DB7C-A9CD-DE46-B639-AE337136AAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -542,12 +542,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -579,7 +585,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
@@ -588,9 +594,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,18 +1005,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="24" max="24" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1080,13 +1089,13 @@
       <c r="X1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="9" t="s">
         <v>25</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="9" t="s">
         <v>27</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -1118,8 +1127,8 @@
       </c>
       <c r="AK1" s="2"/>
     </row>
-    <row r="2" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="5"/>
@@ -1175,13 +1184,13 @@
         <v>2</v>
       </c>
       <c r="X2" s="2"/>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="9" t="s">
         <v>49</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB2" s="2"/>
@@ -1203,8 +1212,8 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="5"/>
@@ -1256,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="X3" s="2"/>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="9" t="s">
         <v>63</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB3" s="2"/>
@@ -1284,8 +1293,8 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="5"/>
@@ -1337,13 +1346,13 @@
         <v>2</v>
       </c>
       <c r="X4" s="2"/>
-      <c r="Y4" s="2" t="s">
+      <c r="Y4" s="9" t="s">
         <v>49</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB4" s="2"/>
@@ -1365,8 +1374,8 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="5"/>
@@ -1422,13 +1431,13 @@
         <v>0</v>
       </c>
       <c r="X5" s="2"/>
-      <c r="Y5" s="2" t="s">
+      <c r="Y5" s="9" t="s">
         <v>74</v>
       </c>
       <c r="Z5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB5" s="2"/>
@@ -1452,8 +1461,8 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="5"/>
@@ -1511,13 +1520,13 @@
         <v>1</v>
       </c>
       <c r="X6" s="2"/>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="9" t="s">
         <v>74</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB6" s="2"/>
@@ -1541,8 +1550,8 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="5"/>
@@ -1598,13 +1607,13 @@
         <v>0</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2" t="s">
+      <c r="Y7" s="9" t="s">
         <v>49</v>
       </c>
       <c r="Z7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB7" s="2"/>
@@ -1626,8 +1635,8 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="5"/>
@@ -1683,13 +1692,13 @@
         <v>3</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2" t="s">
+      <c r="Y8" s="9" t="s">
         <v>74</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB8" s="2"/>
@@ -1711,8 +1720,8 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:37" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="5"/>
@@ -1768,13 +1777,13 @@
         <v>1</v>
       </c>
       <c r="X9" s="2"/>
-      <c r="Y9" s="2" t="s">
+      <c r="Y9" s="9" t="s">
         <v>74</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AB9" s="2"/>
@@ -1796,7 +1805,7 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>95</v>
       </c>
@@ -1881,7 +1890,7 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>103</v>
       </c>
@@ -1966,7 +1975,7 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>109</v>
       </c>
@@ -2059,7 +2068,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>125</v>
       </c>
@@ -2146,7 +2155,7 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>134</v>
       </c>
@@ -2231,7 +2240,7 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>137</v>
       </c>
@@ -2312,7 +2321,7 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>141</v>
       </c>
@@ -2403,7 +2412,7 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>147</v>
       </c>

</xml_diff>